<commit_message>
Investigating gap between rosters and ys results for blackman
</commit_message>
<xml_diff>
--- a/Deliverables/planning.xlsx
+++ b/Deliverables/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A21982-7E8C-4D4D-AD31-00E986997652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6937BEEB-69C9-3943-8B36-86951E6A7EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22500" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22500" windowHeight="20100" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackman Middle School" sheetId="1" r:id="rId1"/>
@@ -2949,7 +2949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:XFD27"/>
     </sheetView>
   </sheetViews>
@@ -5351,7 +5351,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD23"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7793,8 +7793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A208E7-51F2-4750-971F-40A4581FD6A3}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Initial run on Oakland middle complete. Next integrate backfill
</commit_message>
<xml_diff>
--- a/Deliverables/planning.xlsx
+++ b/Deliverables/planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6937BEEB-69C9-3943-8B36-86951E6A7EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E8199F-CB89-E645-B54F-6F34F327EAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="22500" windowHeight="20100" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="22500" windowHeight="20100" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackman Middle School" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="791">
   <si>
     <t>POS</t>
   </si>
@@ -984,9 +984,6 @@
   </si>
   <si>
     <t>https://rcschools.zoom.us/j/83617170903</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auditorium </t>
   </si>
   <si>
     <t>Hearnes</t>
@@ -3423,7 +3420,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3464,19 +3461,19 @@
         <v>800</v>
       </c>
       <c r="C2" s="24" t="s">
+        <v>711</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>712</v>
       </c>
-      <c r="D2" s="23" t="s">
-        <v>713</v>
-      </c>
       <c r="E2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="G2" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -3487,42 +3484,42 @@
         <v>801</v>
       </c>
       <c r="C3" s="24" t="s">
+        <v>713</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>714</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>715</v>
-      </c>
       <c r="E3" t="s">
+        <v>372</v>
+      </c>
+      <c r="F3" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="G3" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B4" s="24">
         <v>802</v>
       </c>
       <c r="C4" s="24" t="s">
+        <v>715</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>716</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>717</v>
-      </c>
       <c r="E4" t="s">
+        <v>379</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="G4" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3533,19 +3530,19 @@
         <v>803</v>
       </c>
       <c r="C5" s="24" t="s">
+        <v>717</v>
+      </c>
+      <c r="D5" s="23" t="s">
         <v>718</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>719</v>
-      </c>
       <c r="E5" t="s">
+        <v>384</v>
+      </c>
+      <c r="F5" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="G5" s="28" t="s">
         <v>386</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -3556,10 +3553,10 @@
         <v>804</v>
       </c>
       <c r="C6" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>720</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>721</v>
       </c>
       <c r="E6" t="s">
         <v>129</v>
@@ -3579,65 +3576,65 @@
         <v>805</v>
       </c>
       <c r="C7" s="24" t="s">
+        <v>721</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>722</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>723</v>
-      </c>
       <c r="E7" t="s">
+        <v>391</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="G7" t="s">
         <v>393</v>
-      </c>
-      <c r="G7" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B8" s="24">
         <v>811</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>723</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>724</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>725</v>
-      </c>
       <c r="E8" t="s">
+        <v>397</v>
+      </c>
+      <c r="F8" s="23" t="s">
         <v>398</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="G8" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B9" s="24">
         <v>807</v>
       </c>
       <c r="C9" s="24" t="s">
+        <v>725</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>726</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>727</v>
-      </c>
       <c r="E9" t="s">
+        <v>403</v>
+      </c>
+      <c r="F9" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="G9" s="23" t="s">
         <v>405</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -3648,19 +3645,19 @@
         <v>808</v>
       </c>
       <c r="C10" s="24" t="s">
+        <v>727</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>728</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>729</v>
-      </c>
       <c r="E10" t="s">
+        <v>408</v>
+      </c>
+      <c r="F10" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="G10" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -3671,19 +3668,19 @@
         <v>214</v>
       </c>
       <c r="C11" s="24" t="s">
+        <v>729</v>
+      </c>
+      <c r="D11" s="23" t="s">
         <v>730</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>731</v>
-      </c>
       <c r="E11" t="s">
+        <v>413</v>
+      </c>
+      <c r="F11" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="G11" t="s">
         <v>415</v>
-      </c>
-      <c r="G11" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3694,19 +3691,19 @@
         <v>806</v>
       </c>
       <c r="C12" s="24" t="s">
+        <v>731</v>
+      </c>
+      <c r="D12" s="23" t="s">
         <v>732</v>
       </c>
-      <c r="D12" s="23" t="s">
-        <v>733</v>
-      </c>
       <c r="E12" t="s">
+        <v>418</v>
+      </c>
+      <c r="F12" s="23" t="s">
         <v>419</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="G12" s="23" t="s">
         <v>420</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -3717,33 +3714,33 @@
         <v>228</v>
       </c>
       <c r="C13" s="24" t="s">
+        <v>733</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>734</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>735</v>
-      </c>
       <c r="E13" t="s">
+        <v>423</v>
+      </c>
+      <c r="F13" s="23" t="s">
         <v>424</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="G13" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B14" s="24">
         <v>810</v>
       </c>
       <c r="C14" s="24" t="s">
+        <v>735</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>736</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>737</v>
       </c>
       <c r="E14" t="s">
         <v>196</v>
@@ -3752,7 +3749,7 @@
         <v>197</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3763,42 +3760,42 @@
         <v>813</v>
       </c>
       <c r="C15" s="24" t="s">
+        <v>737</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>738</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>739</v>
-      </c>
       <c r="E15" t="s">
+        <v>432</v>
+      </c>
+      <c r="F15" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="G15" s="28" t="s">
         <v>434</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B16" s="24">
         <v>700</v>
       </c>
       <c r="C16" s="24" t="s">
+        <v>739</v>
+      </c>
+      <c r="D16" s="23" t="s">
         <v>740</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>741</v>
-      </c>
       <c r="E16" t="s">
+        <v>438</v>
+      </c>
+      <c r="F16" s="23" t="s">
         <v>439</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="G16" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
@@ -3892,19 +3889,19 @@
         <v>107</v>
       </c>
       <c r="C2" t="s">
+        <v>741</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" t="s">
         <v>743</v>
       </c>
-      <c r="E2" t="s">
-        <v>744</v>
-      </c>
       <c r="F2" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -3912,22 +3909,22 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>744</v>
+      </c>
+      <c r="C3" t="s">
         <v>745</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" t="s">
         <v>747</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="4" t="s">
         <v>748</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>749</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -3938,19 +3935,19 @@
         <v>110</v>
       </c>
       <c r="C4" t="s">
+        <v>749</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>751</v>
-      </c>
       <c r="E4" t="s">
+        <v>541</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="22" t="s">
         <v>543</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3961,19 +3958,19 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
+        <v>751</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>752</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>753</v>
-      </c>
       <c r="E5" t="s">
+        <v>546</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -3984,42 +3981,42 @@
         <v>116</v>
       </c>
       <c r="C6" t="s">
+        <v>753</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>755</v>
-      </c>
       <c r="E6" t="s">
+        <v>551</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>553</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B7" t="s">
+        <v>744</v>
+      </c>
+      <c r="C7" t="s">
         <v>745</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>747</v>
-      </c>
       <c r="E7" t="s">
+        <v>557</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>558</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>538</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -4030,42 +4027,42 @@
         <v>116</v>
       </c>
       <c r="C8" t="s">
+        <v>753</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>755</v>
-      </c>
       <c r="E8" t="s">
+        <v>561</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>563</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B9" t="s">
+        <v>744</v>
+      </c>
+      <c r="C9" t="s">
         <v>745</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>747</v>
-      </c>
       <c r="E9" t="s">
+        <v>567</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -4076,65 +4073,65 @@
         <v>107</v>
       </c>
       <c r="C10" t="s">
+        <v>741</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>743</v>
-      </c>
       <c r="E10" t="s">
+        <v>571</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>573</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B11">
         <v>25</v>
       </c>
       <c r="C11" t="s">
+        <v>751</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>752</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>753</v>
-      </c>
       <c r="E11" t="s">
+        <v>576</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" t="s">
         <v>578</v>
-      </c>
-      <c r="G11" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B12">
         <v>116</v>
       </c>
       <c r="C12" t="s">
+        <v>753</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>755</v>
-      </c>
       <c r="E12" t="s">
+        <v>582</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="17" t="s">
         <v>584</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4145,19 +4142,19 @@
         <v>107</v>
       </c>
       <c r="C13" t="s">
+        <v>741</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>743</v>
-      </c>
       <c r="E13" t="s">
+        <v>587</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" t="s">
         <v>589</v>
-      </c>
-      <c r="G13" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -4168,19 +4165,19 @@
         <v>107</v>
       </c>
       <c r="C14" t="s">
+        <v>741</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>742</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>743</v>
-      </c>
       <c r="E14" t="s">
+        <v>592</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>594</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4191,42 +4188,42 @@
         <v>110</v>
       </c>
       <c r="C15" t="s">
+        <v>749</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>751</v>
-      </c>
       <c r="E15" t="s">
+        <v>597</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="2" t="s">
         <v>599</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B16">
         <v>116</v>
       </c>
       <c r="C16" t="s">
+        <v>753</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>754</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>755</v>
-      </c>
       <c r="E16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -4338,8 +4335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91486225-7CD7-4453-82DE-FE7D204837CC}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4382,10 +4379,10 @@
         <v>600</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>756</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>757</v>
       </c>
       <c r="E2" t="s">
         <v>114</v>
@@ -4405,10 +4402,10 @@
         <v>601</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>758</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>759</v>
       </c>
       <c r="E3" t="s">
         <v>114</v>
@@ -4428,10 +4425,10 @@
         <v>602</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>760</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>761</v>
       </c>
       <c r="E4" t="s">
         <v>124</v>
@@ -4451,10 +4448,10 @@
         <v>605</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>762</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>763</v>
       </c>
       <c r="E5" t="s">
         <v>129</v>
@@ -4471,13 +4468,13 @@
         <v>132</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>765</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>766</v>
       </c>
       <c r="E6" t="s">
         <v>135</v>
@@ -4497,10 +4494,10 @@
         <v>214</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>767</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>768</v>
       </c>
       <c r="E7" t="s">
         <v>140</v>
@@ -4520,10 +4517,10 @@
         <v>603</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>769</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>770</v>
       </c>
       <c r="E8" t="s">
         <v>146</v>
@@ -4543,10 +4540,10 @@
         <v>606</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>771</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>772</v>
       </c>
       <c r="E9" t="s">
         <v>151</v>
@@ -4566,10 +4563,10 @@
         <v>607</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>773</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>774</v>
       </c>
       <c r="E10" t="s">
         <v>114</v>
@@ -4589,10 +4586,10 @@
         <v>604</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>775</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>776</v>
       </c>
       <c r="E11" t="s">
         <v>159</v>
@@ -4612,10 +4609,10 @@
         <v>610</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>777</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>778</v>
       </c>
       <c r="E12" t="s">
         <v>164</v>
@@ -4635,10 +4632,10 @@
         <v>609</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>779</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>780</v>
       </c>
       <c r="E13" t="s">
         <v>169</v>
@@ -4658,10 +4655,10 @@
         <v>228</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>781</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>782</v>
       </c>
       <c r="E14" t="s">
         <v>175</v>
@@ -4681,10 +4678,10 @@
         <v>612</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>783</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>784</v>
       </c>
       <c r="E15" t="s">
         <v>181</v>
@@ -4704,10 +4701,10 @@
         <v>611</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>785</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>786</v>
       </c>
       <c r="E16" t="s">
         <v>186</v>
@@ -4727,10 +4724,10 @@
         <v>202</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>787</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>788</v>
       </c>
       <c r="E17" t="s">
         <v>191</v>
@@ -4739,7 +4736,7 @@
         <v>192</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -4750,10 +4747,10 @@
         <v>200</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>790</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>791</v>
       </c>
       <c r="E18" t="s">
         <v>196</v>
@@ -5351,7 +5348,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5707,7 +5704,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD29"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5955,91 +5952,91 @@
         <v>63</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" t="s">
         <v>314</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" t="s">
         <v>316</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>318</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B12">
         <v>702</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" t="s">
         <v>322</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B13">
         <v>703</v>
       </c>
       <c r="C13" t="s">
+        <v>326</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" t="s">
         <v>328</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" t="s">
         <v>330</v>
-      </c>
-      <c r="G13" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B14">
         <v>704</v>
       </c>
       <c r="C14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" t="s">
         <v>334</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" t="s">
         <v>336</v>
-      </c>
-      <c r="G14" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -6050,19 +6047,19 @@
         <v>709</v>
       </c>
       <c r="C15" t="s">
+        <v>337</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" t="s">
         <v>339</v>
-      </c>
-      <c r="E15" t="s">
-        <v>340</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>271</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -6073,19 +6070,19 @@
         <v>706</v>
       </c>
       <c r="C16" t="s">
+        <v>341</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" t="s">
         <v>343</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>345</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -6096,19 +6093,19 @@
         <v>705</v>
       </c>
       <c r="C17" t="s">
+        <v>346</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" t="s">
         <v>348</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" t="s">
         <v>350</v>
-      </c>
-      <c r="G17" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -6119,16 +6116,16 @@
         <v>707</v>
       </c>
       <c r="C18" t="s">
+        <v>351</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>352</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>353</v>
       </c>
       <c r="E18" t="s">
         <v>199</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>200</v>
@@ -6142,19 +6139,19 @@
         <v>701</v>
       </c>
       <c r="C19" t="s">
+        <v>354</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" t="s">
         <v>356</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="G19" t="s">
         <v>358</v>
-      </c>
-      <c r="G19" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -6165,19 +6162,19 @@
         <v>607</v>
       </c>
       <c r="C20" t="s">
+        <v>359</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" t="s">
         <v>361</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="17" t="s">
         <v>363</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -6321,7 +6318,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD27"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6362,22 +6359,22 @@
         <v>98</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" t="s">
         <v>367</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>369</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -6388,42 +6385,42 @@
         <v>806</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" t="s">
         <v>372</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>374</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="C4" s="8" t="s">
         <v>377</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" t="s">
         <v>379</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="4" t="s">
         <v>380</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>381</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -6434,19 +6431,19 @@
         <v>810</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" t="s">
         <v>384</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="28" t="s">
         <v>386</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -6457,10 +6454,10 @@
         <v>812</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>388</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>389</v>
       </c>
       <c r="E6" t="s">
         <v>129</v>
@@ -6480,65 +6477,65 @@
         <v>809</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" t="s">
         <v>391</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" t="s">
         <v>393</v>
-      </c>
-      <c r="G7" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B8" s="8">
         <v>805</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" t="s">
         <v>397</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>399</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B9" s="8">
         <v>803</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E9" t="s">
         <v>403</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="23" t="s">
         <v>405</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -6549,19 +6546,19 @@
         <v>807</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" t="s">
         <v>408</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -6572,19 +6569,19 @@
         <v>801</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" t="s">
         <v>413</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="4" t="s">
         <v>414</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" t="s">
         <v>415</v>
-      </c>
-      <c r="G11" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -6595,19 +6592,19 @@
         <v>808</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="E12" t="s">
         <v>418</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="23" t="s">
         <v>420</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -6618,33 +6615,33 @@
         <v>228</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="E13" t="s">
         <v>423</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B14" s="8">
         <v>811</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="E14" t="s">
         <v>196</v>
@@ -6653,7 +6650,7 @@
         <v>197</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -6664,56 +6661,56 @@
         <v>804</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="E15" t="s">
         <v>432</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="4" t="s">
         <v>433</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="28" t="s">
         <v>434</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B16" s="8">
         <v>802</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>436</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="E16" t="s">
         <v>438</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="C17" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="6" t="s">
         <v>444</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>445</v>
       </c>
       <c r="E17" t="s">
         <v>223</v>
@@ -6728,19 +6725,19 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>448</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -6895,19 +6892,19 @@
         <v>811</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>450</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" t="s">
         <v>451</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
         <v>452</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>453</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -6918,19 +6915,19 @@
         <v>214</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>455</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" t="s">
         <v>456</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="4" t="s">
         <v>457</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>458</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -6941,19 +6938,19 @@
         <v>803</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>460</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" t="s">
         <v>461</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>462</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" s="29" t="s">
         <v>463</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -6964,42 +6961,42 @@
         <v>209</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>465</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" t="s">
         <v>466</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="4" t="s">
         <v>467</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="22" t="s">
         <v>468</v>
-      </c>
-      <c r="G5" s="22" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B6" s="2">
         <v>800</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>471</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" t="s">
         <v>472</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="4" t="s">
         <v>473</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="22" t="s">
         <v>474</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -7010,19 +7007,19 @@
         <v>804</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>476</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" t="s">
         <v>477</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="4" t="s">
         <v>478</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" t="s">
         <v>479</v>
-      </c>
-      <c r="G7" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7033,42 +7030,42 @@
         <v>806</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>481</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" t="s">
         <v>482</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="4" t="s">
         <v>483</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" t="s">
         <v>484</v>
-      </c>
-      <c r="G8" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B9" s="2">
         <v>805</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" t="s">
         <v>488</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="22" t="s">
         <v>490</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7079,42 +7076,42 @@
         <v>812</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" t="s">
         <v>493</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="4" t="s">
         <v>494</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="17" t="s">
         <v>495</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B11" s="2">
         <v>809</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" t="s">
         <v>498</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" t="s">
         <v>500</v>
-      </c>
-      <c r="G11" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -7125,19 +7122,19 @@
         <v>801</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" t="s">
         <v>503</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" t="s">
         <v>505</v>
-      </c>
-      <c r="G12" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -7148,16 +7145,16 @@
         <v>807</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>507</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" t="s">
         <v>508</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="4" t="s">
         <v>509</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>510</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>198</v>
@@ -7171,19 +7168,19 @@
         <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" t="s">
         <v>512</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" t="s">
         <v>514</v>
-      </c>
-      <c r="G14" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -7194,19 +7191,19 @@
         <v>214</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" t="s">
         <v>517</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -7217,19 +7214,19 @@
         <v>810</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" t="s">
         <v>522</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>524</v>
-      </c>
       <c r="G16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -7240,19 +7237,19 @@
         <v>802</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" t="s">
         <v>526</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="22" t="s">
         <v>528</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>529</v>
       </c>
     </row>
   </sheetData>
@@ -7300,7 +7297,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD26"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7345,19 +7342,19 @@
         <v>804</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" t="s">
         <v>531</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -7368,19 +7365,19 @@
         <v>801</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" t="s">
         <v>536</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -7391,19 +7388,19 @@
         <v>807</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" t="s">
         <v>541</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="22" t="s">
         <v>543</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -7414,19 +7411,19 @@
         <v>202</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" t="s">
         <v>546</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7437,42 +7434,42 @@
         <v>205</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" t="s">
         <v>551</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>553</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B7" s="2">
         <v>809</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" t="s">
         <v>557</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>558</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>538</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7483,42 +7480,42 @@
         <v>811</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" t="s">
         <v>561</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>563</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B9" s="2">
         <v>810</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" t="s">
         <v>567</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -7529,65 +7526,65 @@
         <v>812</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="E10" t="s">
         <v>571</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>573</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B11" s="2">
         <v>805</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" t="s">
         <v>576</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" t="s">
         <v>578</v>
-      </c>
-      <c r="G11" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B12" s="2">
         <v>803</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" t="s">
         <v>582</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="17" t="s">
         <v>584</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -7598,19 +7595,19 @@
         <v>207</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" t="s">
         <v>587</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" t="s">
         <v>589</v>
-      </c>
-      <c r="G13" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -7621,19 +7618,19 @@
         <v>220</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" t="s">
         <v>592</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>594</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -7644,42 +7641,42 @@
         <v>806</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" t="s">
         <v>597</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="2" t="s">
         <v>599</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>214</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" t="s">
         <v>603</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -7793,7 +7790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A208E7-51F2-4750-971F-40A4581FD6A3}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -7839,19 +7836,19 @@
         <v>203</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>606</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>607</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" t="s">
         <v>608</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="17" t="s">
         <v>610</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -7862,19 +7859,19 @@
         <v>204</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>612</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" t="s">
         <v>613</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="17" t="s">
         <v>615</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -7885,42 +7882,42 @@
         <v>207</v>
       </c>
       <c r="C4" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>617</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" t="s">
         <v>618</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="22" t="s">
         <v>620</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B5" s="8">
         <v>111</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>622</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>623</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" t="s">
         <v>624</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="17" t="s">
         <v>626</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -7931,42 +7928,42 @@
         <v>304</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>627</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>628</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" t="s">
         <v>629</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="17" t="s">
         <v>631</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B7" s="8">
         <v>701</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>633</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="E7" t="s">
         <v>634</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="4" t="s">
         <v>635</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>636</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -7977,19 +7974,19 @@
         <v>807</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>637</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>638</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" t="s">
         <v>639</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="17" t="s">
         <v>641</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -8000,19 +7997,19 @@
         <v>402</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>642</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>643</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" t="s">
         <v>644</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>646</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -8023,19 +8020,19 @@
         <v>107</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>648</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" t="s">
         <v>649</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="4" t="s">
         <v>650</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>651</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -8046,19 +8043,19 @@
         <v>214</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>652</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>653</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" t="s">
         <v>654</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>656</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -8069,111 +8066,111 @@
         <v>228</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>658</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" t="s">
         <v>659</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="17" t="s">
         <v>661</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B13" s="8">
         <v>105</v>
       </c>
       <c r="C13" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>664</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" t="s">
         <v>665</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="2" t="s">
         <v>667</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B14" s="8">
         <v>306</v>
       </c>
       <c r="C14" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>669</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" t="s">
         <v>670</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="2" t="s">
         <v>672</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B15" s="8">
         <v>606</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>674</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>675</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>676</v>
-      </c>
       <c r="E15" t="s">
+        <v>582</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="17" t="s">
         <v>584</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B16" s="8">
         <v>308</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>677</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>678</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" t="s">
         <v>679</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="4" t="s">
         <v>680</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="2" t="s">
         <v>681</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>682</v>
       </c>
     </row>
   </sheetData>
@@ -8218,7 +8215,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD27"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8261,19 +8258,19 @@
         <v>615</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E2" t="s">
+        <v>531</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -8284,19 +8281,19 @@
         <v>500</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>683</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>684</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>685</v>
-      </c>
       <c r="E3" t="s">
+        <v>536</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>538</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -8307,19 +8304,19 @@
         <v>502</v>
       </c>
       <c r="C4" s="11" t="s">
+        <v>685</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>686</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>687</v>
-      </c>
       <c r="E4" t="s">
+        <v>541</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="22" t="s">
         <v>543</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -8330,19 +8327,19 @@
         <v>607</v>
       </c>
       <c r="C5" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>688</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>689</v>
-      </c>
       <c r="E5" t="s">
+        <v>546</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -8353,42 +8350,42 @@
         <v>601</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>689</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>690</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>691</v>
-      </c>
       <c r="E6" t="s">
+        <v>551</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>553</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B7" s="11">
         <v>609</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>692</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>693</v>
-      </c>
       <c r="E7" t="s">
+        <v>557</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>558</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>538</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -8399,42 +8396,42 @@
         <v>611</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>693</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>694</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>695</v>
-      </c>
       <c r="E8" t="s">
+        <v>561</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>563</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B9" s="11">
         <v>613</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>695</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>696</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>697</v>
-      </c>
       <c r="E9" t="s">
+        <v>567</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -8445,65 +8442,65 @@
         <v>605</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>697</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>698</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>699</v>
-      </c>
       <c r="E10" t="s">
+        <v>571</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="G10" s="4" t="s">
         <v>573</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B11" s="11">
         <v>614</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>699</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>700</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>701</v>
-      </c>
       <c r="E11" t="s">
+        <v>576</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" t="s">
         <v>578</v>
-      </c>
-      <c r="G11" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B12" s="11">
         <v>612</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>701</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>702</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>703</v>
-      </c>
       <c r="E12" t="s">
+        <v>582</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>583</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="17" t="s">
         <v>584</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -8514,19 +8511,19 @@
         <v>610</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>703</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>704</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>705</v>
-      </c>
       <c r="E13" t="s">
+        <v>587</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>588</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" t="s">
         <v>589</v>
-      </c>
-      <c r="G13" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -8537,19 +8534,19 @@
         <v>606</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>705</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>706</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>707</v>
-      </c>
       <c r="E14" t="s">
+        <v>592</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>594</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -8560,42 +8557,42 @@
         <v>603</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>707</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>708</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>709</v>
-      </c>
       <c r="E15" t="s">
+        <v>597</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="2" t="s">
         <v>599</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>214</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>709</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>710</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>711</v>
-      </c>
       <c r="E16" t="s">
+        <v>603</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="21" spans="7:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Beta refactoring complete. Awaiting updated docs from county.
</commit_message>
<xml_diff>
--- a/Deliverables/planning.xlsx
+++ b/Deliverables/planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Desktop/From RuCo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111B94F0-9DD6-B344-9D1D-274498A0F894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0223643F-24AF-1644-8C6F-AEF7154C2CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackman Middle School" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="372">
   <si>
     <t>MS Room Number</t>
   </si>
@@ -1146,16 +1146,19 @@
     <t>skeltonc@rcschools.net</t>
   </si>
   <si>
-    <t>202 (if needed)</t>
-  </si>
-  <si>
-    <t>205 (if needed)</t>
-  </si>
-  <si>
-    <t>220 (if needed)</t>
-  </si>
-  <si>
     <t>Auditorium (if needed)</t>
+  </si>
+  <si>
+    <t>Fake 1</t>
+  </si>
+  <si>
+    <t>Fake 2</t>
+  </si>
+  <si>
+    <t>Fake 3</t>
+  </si>
+  <si>
+    <t>Fake 4</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1385,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1670,7 +1673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3867,10 +3870,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59636EF-7029-413B-81DF-F480CA3050FB}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4050,8 +4053,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>367</v>
+      <c r="A13">
+        <v>202</v>
       </c>
       <c r="B13" t="s">
         <v>241</v>
@@ -4061,8 +4064,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>368</v>
+      <c r="A14">
+        <v>205</v>
       </c>
       <c r="B14" t="s">
         <v>241</v>
@@ -4072,13 +4075,21 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>369</v>
+      <c r="A15">
+        <v>220</v>
       </c>
       <c r="B15" t="s">
         <v>241</v>
       </c>
       <c r="D15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>368</v>
+      </c>
+      <c r="D16">
         <v>30</v>
       </c>
     </row>
@@ -4102,10 +4113,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4933BC48-B205-4C59-821F-2A2E73CA6687}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4338,6 +4349,38 @@
       </c>
       <c r="D16" s="7">
         <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D17" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="D18" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="D19" s="7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D20" s="7">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4370,7 +4413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29AB360-CA70-42CD-A478-E3B9B19FB8F8}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -4622,7 +4665,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>

</xml_diff>

<commit_message>
Updated capacity report and prepped for 2023 run.
</commit_message>
<xml_diff>
--- a/Deliverables/planning.xlsx
+++ b/Deliverables/planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0223643F-24AF-1644-8C6F-AEF7154C2CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CE1800-BA0A-0B49-B0F7-0924B4D4F959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4960" yWindow="5400" windowWidth="19020" windowHeight="14240" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackman Middle School" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="399">
   <si>
     <t>MS Room Number</t>
   </si>
@@ -342,9 +342,6 @@
     <t>houlef@rcschools.net</t>
   </si>
   <si>
-    <t>Library (if needed)</t>
-  </si>
-  <si>
     <t>Willis, Cheryl</t>
   </si>
   <si>
@@ -1146,19 +1143,103 @@
     <t>skeltonc@rcschools.net</t>
   </si>
   <si>
-    <t>Auditorium (if needed)</t>
-  </si>
-  <si>
-    <t>Fake 1</t>
-  </si>
-  <si>
-    <t>Fake 2</t>
-  </si>
-  <si>
-    <t>Fake 3</t>
-  </si>
-  <si>
-    <t>Fake 4</t>
+    <t>Sean Kirkpatrick</t>
+  </si>
+  <si>
+    <t>kirkpatricks@rcschools.net</t>
+  </si>
+  <si>
+    <t>Ruth-Ann Logsdon</t>
+  </si>
+  <si>
+    <t>logsdonr@rcschools.net</t>
+  </si>
+  <si>
+    <t>Lily Parker</t>
+  </si>
+  <si>
+    <t>parkerl@rcschools.net</t>
+  </si>
+  <si>
+    <t>Sarah Schwartz</t>
+  </si>
+  <si>
+    <t>schwartzs@rcschools.net</t>
+  </si>
+  <si>
+    <t>Mark Stirbens</t>
+  </si>
+  <si>
+    <t>stirbensm@rcschools.net</t>
+  </si>
+  <si>
+    <t>Stephanie Jones </t>
+  </si>
+  <si>
+    <t>joness@rcschools.net</t>
+  </si>
+  <si>
+    <t>Kevin Laterza</t>
+  </si>
+  <si>
+    <t>laterzak@rcschools.net</t>
+  </si>
+  <si>
+    <t>Dakota Gentry</t>
+  </si>
+  <si>
+    <t>gentryh@rcschools.net</t>
+  </si>
+  <si>
+    <t>Cameron Medina</t>
+  </si>
+  <si>
+    <t>Elena Clemons</t>
+  </si>
+  <si>
+    <t>clemonse@rcschools.net</t>
+  </si>
+  <si>
+    <t>Anna Dicus</t>
+  </si>
+  <si>
+    <t>dicusa@rcschools.net</t>
+  </si>
+  <si>
+    <t>Samantha Reves</t>
+  </si>
+  <si>
+    <t>revess@rcschools.net</t>
+  </si>
+  <si>
+    <t>Jessica Logan</t>
+  </si>
+  <si>
+    <t>loganj@rcschools.net</t>
+  </si>
+  <si>
+    <t>Cedric Roberts</t>
+  </si>
+  <si>
+    <t>robertsc@rcschools.net</t>
+  </si>
+  <si>
+    <t>Shannon Minner</t>
+  </si>
+  <si>
+    <t>New Hire, no email yet</t>
+  </si>
+  <si>
+    <t>Janice Penny</t>
+  </si>
+  <si>
+    <t>pennyj@rcschools.net</t>
+  </si>
+  <si>
+    <t>Valori Bonds</t>
+  </si>
+  <si>
+    <t>bondsv@rcschools.net</t>
   </si>
 </sst>
 </file>
@@ -1193,6 +1274,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -2070,10 +2152,10 @@
         <v>800</v>
       </c>
       <c r="B2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>304</v>
       </c>
       <c r="D2">
         <v>25</v>
@@ -2084,10 +2166,10 @@
         <v>801</v>
       </c>
       <c r="B3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -2098,10 +2180,10 @@
         <v>802</v>
       </c>
       <c r="B4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>307</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>308</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -2112,10 +2194,10 @@
         <v>803</v>
       </c>
       <c r="B5" t="s">
+        <v>308</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -2126,10 +2208,10 @@
         <v>804</v>
       </c>
       <c r="B6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="D6">
         <v>25</v>
@@ -2140,10 +2222,10 @@
         <v>805</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D7">
         <v>25</v>
@@ -2154,10 +2236,10 @@
         <v>806</v>
       </c>
       <c r="B8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="D8">
         <v>25</v>
@@ -2168,10 +2250,10 @@
         <v>807</v>
       </c>
       <c r="B9" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>317</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -2182,10 +2264,10 @@
         <v>808</v>
       </c>
       <c r="B10" t="s">
+        <v>317</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>319</v>
       </c>
       <c r="D10">
         <v>25</v>
@@ -2196,10 +2278,10 @@
         <v>810</v>
       </c>
       <c r="B11" t="s">
+        <v>319</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -2210,10 +2292,10 @@
         <v>811</v>
       </c>
       <c r="B12" t="s">
+        <v>321</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -2224,10 +2306,10 @@
         <v>812</v>
       </c>
       <c r="B13" t="s">
+        <v>323</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>325</v>
       </c>
       <c r="D13">
         <v>25</v>
@@ -2235,13 +2317,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" t="s">
         <v>326</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="2" t="s">
         <v>327</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>328</v>
       </c>
       <c r="D14">
         <v>25</v>
@@ -2249,13 +2331,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s">
+        <v>328</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="D15">
         <v>25</v>
@@ -2263,13 +2345,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" t="s">
+        <v>330</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>332</v>
       </c>
       <c r="D16">
         <v>40</v>
@@ -2332,10 +2414,10 @@
         <v>600</v>
       </c>
       <c r="B2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>333</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>334</v>
       </c>
       <c r="D2">
         <v>25</v>
@@ -2346,10 +2428,10 @@
         <v>601</v>
       </c>
       <c r="B3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>336</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -2360,10 +2442,10 @@
         <v>602</v>
       </c>
       <c r="B4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>337</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>338</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -2374,10 +2456,10 @@
         <v>603</v>
       </c>
       <c r="B5" t="s">
+        <v>338</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>340</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -2388,10 +2470,10 @@
         <v>604</v>
       </c>
       <c r="B6" t="s">
+        <v>340</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>342</v>
       </c>
       <c r="D6">
         <v>25</v>
@@ -2402,10 +2484,10 @@
         <v>605</v>
       </c>
       <c r="B7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="D7">
         <v>25</v>
@@ -2416,10 +2498,10 @@
         <v>606</v>
       </c>
       <c r="B8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="D8">
         <v>25</v>
@@ -2430,10 +2512,10 @@
         <v>607</v>
       </c>
       <c r="B9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="D9">
         <v>25</v>
@@ -2444,10 +2526,10 @@
         <v>609</v>
       </c>
       <c r="B10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>350</v>
       </c>
       <c r="D10">
         <v>25</v>
@@ -2458,10 +2540,10 @@
         <v>610</v>
       </c>
       <c r="B11" t="s">
+        <v>350</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>352</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -2472,10 +2554,10 @@
         <v>611</v>
       </c>
       <c r="B12" t="s">
+        <v>352</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -2486,10 +2568,10 @@
         <v>612</v>
       </c>
       <c r="B13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="D13">
         <v>25</v>
@@ -2500,10 +2582,10 @@
         <v>200</v>
       </c>
       <c r="B14" t="s">
+        <v>356</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="D14">
         <v>25</v>
@@ -2514,10 +2596,10 @@
         <v>202</v>
       </c>
       <c r="B15" t="s">
+        <v>358</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="D15">
         <v>25</v>
@@ -2528,10 +2610,10 @@
         <v>207</v>
       </c>
       <c r="B16" t="s">
+        <v>360</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="D16">
         <v>10</v>
@@ -2539,13 +2621,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B17" t="s">
+        <v>362</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>364</v>
       </c>
       <c r="D17">
         <v>30</v>
@@ -2553,13 +2635,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B18" t="s">
+        <v>364</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="D18">
         <v>50</v>
@@ -2591,10 +2673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A2421DD-75DC-4CD7-BE15-0A38EEB98C35}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2619,6 +2701,241 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>800</v>
+      </c>
+      <c r="B2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>801</v>
+      </c>
+      <c r="B3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>802</v>
+      </c>
+      <c r="B4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>803</v>
+      </c>
+      <c r="B5" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>804</v>
+      </c>
+      <c r="B6" t="s">
+        <v>374</v>
+      </c>
+      <c r="C6" t="s">
+        <v>375</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>805</v>
+      </c>
+      <c r="B7" t="s">
+        <v>376</v>
+      </c>
+      <c r="C7" t="s">
+        <v>377</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>806</v>
+      </c>
+      <c r="B8" t="s">
+        <v>378</v>
+      </c>
+      <c r="C8" t="s">
+        <v>379</v>
+      </c>
+      <c r="D8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>807</v>
+      </c>
+      <c r="B9" t="s">
+        <v>380</v>
+      </c>
+      <c r="C9" t="s">
+        <v>381</v>
+      </c>
+      <c r="D9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>808</v>
+      </c>
+      <c r="B10" t="s">
+        <v>382</v>
+      </c>
+      <c r="D10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>809</v>
+      </c>
+      <c r="B11" t="s">
+        <v>383</v>
+      </c>
+      <c r="C11" t="s">
+        <v>384</v>
+      </c>
+      <c r="D11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>810</v>
+      </c>
+      <c r="B12" t="s">
+        <v>385</v>
+      </c>
+      <c r="C12" t="s">
+        <v>386</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>811</v>
+      </c>
+      <c r="B13" t="s">
+        <v>387</v>
+      </c>
+      <c r="C13" t="s">
+        <v>388</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>812</v>
+      </c>
+      <c r="B14" t="s">
+        <v>389</v>
+      </c>
+      <c r="C14" t="s">
+        <v>390</v>
+      </c>
+      <c r="D14">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>700</v>
+      </c>
+      <c r="B15" t="s">
+        <v>391</v>
+      </c>
+      <c r="C15" t="s">
+        <v>392</v>
+      </c>
+      <c r="D15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>200</v>
+      </c>
+      <c r="B16" t="s">
+        <v>393</v>
+      </c>
+      <c r="C16" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>301</v>
+      </c>
+      <c r="B17" t="s">
+        <v>395</v>
+      </c>
+      <c r="C17" t="s">
+        <v>396</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>407</v>
+      </c>
+      <c r="B18" t="s">
+        <v>397</v>
+      </c>
+      <c r="C18" t="s">
+        <v>398</v>
+      </c>
+      <c r="D18">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2629,7 +2946,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2880,13 +3197,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B18" t="s">
         <v>99</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="D18" s="7">
         <v>50</v>
@@ -2951,10 +3268,10 @@
         <v>600</v>
       </c>
       <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="D2">
         <v>25</v>
@@ -2965,10 +3282,10 @@
         <v>602</v>
       </c>
       <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="D3">
         <v>25</v>
@@ -2979,10 +3296,10 @@
         <v>605</v>
       </c>
       <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="D4">
         <v>25</v>
@@ -2993,10 +3310,10 @@
         <v>604</v>
       </c>
       <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D5">
         <v>25</v>
@@ -3007,10 +3324,10 @@
         <v>611</v>
       </c>
       <c r="B6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="D6">
         <v>25</v>
@@ -3021,10 +3338,10 @@
         <v>613</v>
       </c>
       <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="D7">
         <v>25</v>
@@ -3035,10 +3352,10 @@
         <v>700</v>
       </c>
       <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="D8">
         <v>25</v>
@@ -3049,10 +3366,10 @@
         <v>701</v>
       </c>
       <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -3063,10 +3380,10 @@
         <v>702</v>
       </c>
       <c r="B10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="D10">
         <v>25</v>
@@ -3077,10 +3394,10 @@
         <v>703</v>
       </c>
       <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="D11">
         <v>25</v>
@@ -3091,10 +3408,10 @@
         <v>704</v>
       </c>
       <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="D12">
         <v>25</v>
@@ -3105,10 +3422,10 @@
         <v>705</v>
       </c>
       <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="D13">
         <v>25</v>
@@ -3119,10 +3436,10 @@
         <v>706</v>
       </c>
       <c r="B14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="D14">
         <v>25</v>
@@ -3133,10 +3450,10 @@
         <v>707</v>
       </c>
       <c r="B15" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="D15">
         <v>25</v>
@@ -3147,10 +3464,10 @@
         <v>709</v>
       </c>
       <c r="B16" t="s">
+        <v>129</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="D16">
         <v>25</v>
@@ -3161,10 +3478,10 @@
         <v>710</v>
       </c>
       <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="D17">
         <v>25</v>
@@ -3175,10 +3492,10 @@
         <v>711</v>
       </c>
       <c r="B18" t="s">
+        <v>133</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="D18">
         <v>25</v>
@@ -3189,10 +3506,10 @@
         <v>712</v>
       </c>
       <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="D19">
         <v>25</v>
@@ -3200,13 +3517,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>139</v>
       </c>
       <c r="D20">
         <v>40</v>
@@ -3274,10 +3591,10 @@
         <v>801</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>140</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>141</v>
       </c>
       <c r="D2" s="3">
         <v>25</v>
@@ -3288,10 +3605,10 @@
         <v>802</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>142</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>143</v>
       </c>
       <c r="D3" s="3">
         <v>25</v>
@@ -3302,10 +3619,10 @@
         <v>803</v>
       </c>
       <c r="B4" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="19" t="s">
         <v>144</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>145</v>
       </c>
       <c r="D4" s="3">
         <v>25</v>
@@ -3316,10 +3633,10 @@
         <v>804</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>146</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>147</v>
       </c>
       <c r="D5" s="3">
         <v>25</v>
@@ -3330,10 +3647,10 @@
         <v>805</v>
       </c>
       <c r="B6" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>149</v>
       </c>
       <c r="D6" s="3">
         <v>25</v>
@@ -3344,10 +3661,10 @@
         <v>806</v>
       </c>
       <c r="B7" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>150</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>151</v>
       </c>
       <c r="D7" s="3">
         <v>25</v>
@@ -3358,10 +3675,10 @@
         <v>807</v>
       </c>
       <c r="B8" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>152</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>153</v>
       </c>
       <c r="D8" s="3">
         <v>25</v>
@@ -3372,10 +3689,10 @@
         <v>808</v>
       </c>
       <c r="B9" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>154</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>155</v>
       </c>
       <c r="D9" s="3">
         <v>25</v>
@@ -3386,10 +3703,10 @@
         <v>809</v>
       </c>
       <c r="B10" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="19" t="s">
         <v>156</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>157</v>
       </c>
       <c r="D10" s="3">
         <v>25</v>
@@ -3400,10 +3717,10 @@
         <v>810</v>
       </c>
       <c r="B11" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="19" t="s">
         <v>158</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>159</v>
       </c>
       <c r="D11" s="3">
         <v>25</v>
@@ -3414,10 +3731,10 @@
         <v>811</v>
       </c>
       <c r="B12" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>160</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>161</v>
       </c>
       <c r="D12" s="3">
         <v>25</v>
@@ -3428,10 +3745,10 @@
         <v>812</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>162</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>163</v>
       </c>
       <c r="D13" s="3">
         <v>25</v>
@@ -3442,10 +3759,10 @@
         <v>814</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="D14" s="3">
         <v>25</v>
@@ -3453,13 +3770,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>168</v>
       </c>
       <c r="D15" s="3">
         <v>50</v>
@@ -3467,13 +3784,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>171</v>
       </c>
       <c r="D16" s="3">
         <v>50</v>
@@ -3481,13 +3798,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="C17" s="19" t="s">
         <v>173</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>174</v>
       </c>
       <c r="D17" s="3">
         <v>25</v>
@@ -3548,13 +3865,13 @@
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D2" s="17">
         <v>50</v>
@@ -3562,13 +3879,13 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>178</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>179</v>
       </c>
       <c r="D3" s="17">
         <v>40</v>
@@ -3579,10 +3896,10 @@
         <v>800</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>181</v>
       </c>
       <c r="D4" s="17">
         <v>40</v>
@@ -3593,10 +3910,10 @@
         <v>801</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="D5" s="17">
         <v>40</v>
@@ -3607,10 +3924,10 @@
         <v>802</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>184</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>185</v>
       </c>
       <c r="D6" s="17">
         <v>40</v>
@@ -3621,10 +3938,10 @@
         <v>803</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>186</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>187</v>
       </c>
       <c r="D7" s="17">
         <v>40</v>
@@ -3635,10 +3952,10 @@
         <v>804</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>188</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="D8" s="17">
         <v>40</v>
@@ -3649,10 +3966,10 @@
         <v>805</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>190</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>191</v>
       </c>
       <c r="D9" s="17">
         <v>52</v>
@@ -3663,10 +3980,10 @@
         <v>806</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>193</v>
       </c>
       <c r="D10" s="17">
         <v>40</v>
@@ -3677,10 +3994,10 @@
         <v>807</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>194</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>195</v>
       </c>
       <c r="D11" s="17">
         <v>55</v>
@@ -3691,10 +4008,10 @@
         <v>809</v>
       </c>
       <c r="B12" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>196</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>197</v>
       </c>
       <c r="D12" s="17">
         <v>40</v>
@@ -3705,10 +4022,10 @@
         <v>810</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>198</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>199</v>
       </c>
       <c r="D13" s="17">
         <v>40</v>
@@ -3719,10 +4036,10 @@
         <v>811</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>200</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>201</v>
       </c>
       <c r="D14" s="17">
         <v>40</v>
@@ -3733,10 +4050,10 @@
         <v>812</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>202</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>203</v>
       </c>
       <c r="D15" s="17">
         <v>40</v>
@@ -3747,10 +4064,10 @@
         <v>813</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>204</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>205</v>
       </c>
       <c r="D16" s="17">
         <v>40</v>
@@ -3761,10 +4078,10 @@
         <v>814</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>207</v>
       </c>
       <c r="D17" s="17">
         <v>40</v>
@@ -3775,10 +4092,10 @@
         <v>815</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>208</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>209</v>
       </c>
       <c r="D18" s="17">
         <v>40</v>
@@ -3789,10 +4106,10 @@
         <v>816</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="D19" s="17">
         <v>40</v>
@@ -3803,10 +4120,10 @@
         <v>819</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>213</v>
       </c>
       <c r="D20" s="17">
         <v>40</v>
@@ -3817,10 +4134,10 @@
         <v>820</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>214</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>215</v>
       </c>
       <c r="D21" s="17">
         <v>40</v>
@@ -3828,13 +4145,13 @@
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>217</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>218</v>
       </c>
       <c r="D22" s="18">
         <v>60</v>
@@ -3870,10 +4187,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59636EF-7029-413B-81DF-F480CA3050FB}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3903,10 +4220,10 @@
         <v>803</v>
       </c>
       <c r="B2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="D2">
         <v>30</v>
@@ -3917,10 +4234,10 @@
         <v>810</v>
       </c>
       <c r="B3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="D3">
         <v>30</v>
@@ -3931,10 +4248,10 @@
         <v>804</v>
       </c>
       <c r="B4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>223</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>224</v>
       </c>
       <c r="D4">
         <v>30</v>
@@ -3945,10 +4262,10 @@
         <v>805</v>
       </c>
       <c r="B5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="D5">
         <v>30</v>
@@ -3959,10 +4276,10 @@
         <v>807</v>
       </c>
       <c r="B6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>228</v>
       </c>
       <c r="D6">
         <v>30</v>
@@ -3973,10 +4290,10 @@
         <v>801</v>
       </c>
       <c r="B7" t="s">
+        <v>228</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="D7">
         <v>30</v>
@@ -3987,10 +4304,10 @@
         <v>809</v>
       </c>
       <c r="B8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="D8">
         <v>30</v>
@@ -4001,10 +4318,10 @@
         <v>811</v>
       </c>
       <c r="B9" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>233</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>234</v>
       </c>
       <c r="D9">
         <v>30</v>
@@ -4015,10 +4332,10 @@
         <v>812</v>
       </c>
       <c r="B10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="D10">
         <v>30</v>
@@ -4029,10 +4346,10 @@
         <v>806</v>
       </c>
       <c r="B11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="D11">
         <v>30</v>
@@ -4040,13 +4357,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B12" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>240</v>
       </c>
       <c r="D12">
         <v>40</v>
@@ -4057,7 +4374,7 @@
         <v>202</v>
       </c>
       <c r="B13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D13">
         <v>30</v>
@@ -4068,7 +4385,7 @@
         <v>205</v>
       </c>
       <c r="B14" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D14">
         <v>30</v>
@@ -4079,17 +4396,9 @@
         <v>220</v>
       </c>
       <c r="B15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>368</v>
-      </c>
-      <c r="D16">
         <v>30</v>
       </c>
     </row>
@@ -4113,10 +4422,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4933BC48-B205-4C59-821F-2A2E73CA6687}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4146,10 +4455,10 @@
         <v>511</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="D2" s="7">
         <v>30</v>
@@ -4160,10 +4469,10 @@
         <v>105</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>245</v>
       </c>
       <c r="D3" s="7">
         <v>35</v>
@@ -4174,10 +4483,10 @@
         <v>107</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>247</v>
       </c>
       <c r="D4" s="7">
         <v>35</v>
@@ -4188,10 +4497,10 @@
         <v>203</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>248</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>249</v>
       </c>
       <c r="D5" s="7">
         <v>35</v>
@@ -4202,10 +4511,10 @@
         <v>204</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="D6" s="7">
         <v>35</v>
@@ -4216,10 +4525,10 @@
         <v>304</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>253</v>
       </c>
       <c r="D7" s="7">
         <v>35</v>
@@ -4230,10 +4539,10 @@
         <v>306</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>254</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>255</v>
       </c>
       <c r="D8" s="7">
         <v>35</v>
@@ -4244,10 +4553,10 @@
         <v>402</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="D9" s="7">
         <v>35</v>
@@ -4258,10 +4567,10 @@
         <v>606</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>259</v>
       </c>
       <c r="D10" s="7">
         <v>35</v>
@@ -4272,10 +4581,10 @@
         <v>701</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="D11" s="7">
         <v>35</v>
@@ -4286,10 +4595,10 @@
         <v>111</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="D12" s="7">
         <v>50</v>
@@ -4300,10 +4609,10 @@
         <v>207</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="D13" s="7">
         <v>50</v>
@@ -4314,10 +4623,10 @@
         <v>308</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>266</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="D14" s="7">
         <v>50</v>
@@ -4325,13 +4634,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>268</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="D15" s="7">
         <v>60</v>
@@ -4339,48 +4648,16 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="D16" s="7">
         <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="D17" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="D18" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="D19" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="D20" s="7">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4414,7 +4691,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4441,13 +4718,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>273</v>
       </c>
       <c r="D2" s="3">
         <v>40</v>
@@ -4458,10 +4735,10 @@
         <v>500</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>275</v>
       </c>
       <c r="D3" s="3">
         <v>30</v>
@@ -4472,10 +4749,10 @@
         <v>502</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>277</v>
       </c>
       <c r="D4" s="3">
         <v>30</v>
@@ -4486,10 +4763,10 @@
         <v>601</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>279</v>
       </c>
       <c r="D5" s="3">
         <v>30</v>
@@ -4500,10 +4777,10 @@
         <v>603</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>281</v>
       </c>
       <c r="D6" s="3">
         <v>30</v>
@@ -4514,10 +4791,10 @@
         <v>605</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>283</v>
       </c>
       <c r="D7" s="3">
         <v>30</v>
@@ -4528,10 +4805,10 @@
         <v>606</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>285</v>
       </c>
       <c r="D8" s="3">
         <v>30</v>
@@ -4542,10 +4819,10 @@
         <v>607</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>287</v>
       </c>
       <c r="D9" s="3">
         <v>30</v>
@@ -4556,10 +4833,10 @@
         <v>609</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>288</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>289</v>
       </c>
       <c r="D10" s="3">
         <v>30</v>
@@ -4570,10 +4847,10 @@
         <v>610</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>291</v>
       </c>
       <c r="D11" s="3">
         <v>30</v>
@@ -4584,10 +4861,10 @@
         <v>611</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>293</v>
       </c>
       <c r="D12" s="3">
         <v>30</v>
@@ -4598,10 +4875,10 @@
         <v>612</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>295</v>
       </c>
       <c r="D13" s="3">
         <v>30</v>
@@ -4612,10 +4889,10 @@
         <v>613</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>296</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>297</v>
       </c>
       <c r="D14" s="3">
         <v>10</v>
@@ -4626,10 +4903,10 @@
         <v>614</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>298</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>299</v>
       </c>
       <c r="D15" s="3">
         <v>30</v>
@@ -4643,7 +4920,7 @@
         <v>38</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D16" s="21">
         <v>10</v>
@@ -4654,10 +4931,10 @@
         <v>616</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>301</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="D17" s="3">
         <v>10</v>
@@ -4665,7 +4942,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>367</v>
+        <v>165</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>

</xml_diff>

<commit_message>
Implementing bug fixes: repeated pathways in backfill, the lavergne case
</commit_message>
<xml_diff>
--- a/Deliverables/planning.xlsx
+++ b/Deliverables/planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amurphy/Documents/GitHub/YouScience/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612692EA-22DE-0141-B5F6-EA5A8D14D113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99983EA2-B8D3-D943-B178-92AABE29FADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13420" yWindow="2100" windowWidth="19020" windowHeight="14240" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13420" yWindow="2100" windowWidth="19020" windowHeight="14240" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blackman Middle School" sheetId="1" r:id="rId1"/>
@@ -1399,7 +1399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1445,6 +1445,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1464,7 +1469,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1752,7 +1757,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2942,8 +2947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D970F54-250C-4753-A1A7-C730FC0ACD9B}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2968,88 +2973,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    <row r="2" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
         <v>612</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="D2" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
         <v>611</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="D3" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
         <v>610</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+      <c r="D4" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
         <v>609</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+      <c r="D5" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
         <v>608</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+      <c r="D6" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25">
         <v>607</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="7">
-        <v>25</v>
+      <c r="D7" s="25">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3556,7 +3561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0F0E64-7B56-4590-A08D-4AF2544381B8}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>

</xml_diff>